<commit_message>
update main files dir
</commit_message>
<xml_diff>
--- a/TIMES-NZ/BY_Trans.xlsx
+++ b/TIMES-NZ/BY_Trans.xlsx
@@ -7,9 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BY_Trans" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="FILL Table" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="NCAP_BND" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ImportSettings" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -48,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -415,291 +417,288 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>~TFM_INS</t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ReEnableBYInvestment</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Overrides Veda default settings which usually disable investment in BY techs</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TimeSlice</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+          <t>~TFM_INS</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Attribute</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>attribu_cond</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PSet_Pn</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>LimType</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>RESID</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>BanSelectedBaseYearTechs</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Ensures no investment in selected baseyear techs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>~TFM_INS</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Attribute</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PSet_PN</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>Year</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>AllRegions</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>REG1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>REG2</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Pset_Set</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Pset_PN</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Pset_PD</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Pset_CI</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Pset_CO</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Cset_Set</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Cset_CN</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Cset_CD</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>~TFM_FILL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Operation_Sum_Avg_Count</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Scenario Name</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>TimeSlice</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>LimType</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Attribute</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Other_Indexes</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Tech_Comm_Info</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>AllRegions</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>REG1</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>REG2</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Pset_Set</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Pset_PN</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>~TFM_INS</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TimeSlice</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>LimType</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Attribute</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>AllRegions</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>REG1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>REG2</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Pset_Set</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Pset_PN</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Pset_PD</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Pset_CI</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Pset_CO</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Cset_Set</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Cset_CN</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Cset_CD</t>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ELC_*</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>RES*COA**</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RES*WOD*</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>T_F*PET*</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>T_P_B*PET*</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>T_P_B*LPG*</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>C_WSR-*-DirectH-GEO</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>

</xml_diff>